<commit_message>
added values for fujichrome velvia 50
</commit_message>
<xml_diff>
--- a/schwarzschild.xlsx
+++ b/schwarzschild.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff\Documents\git\multiexposure_schwarzschild_compensation_sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3D8853-FEA0-4DD5-8FF7-95B70041F167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA9E812-2C26-4D98-97BD-3B008B14F683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14746" xr2:uid="{DD76BD61-53DE-40D6-8FFC-6C111A3C2BD9}"/>
+    <workbookView xWindow="18592" yWindow="1230" windowWidth="7666" windowHeight="6000" xr2:uid="{DD76BD61-53DE-40D6-8FFC-6C111A3C2BD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,29 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>Exposure (Log H Lux Seconds)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -64,8 +83,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -380,12 +401,188 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99AC11BD-D6EE-45A1-9AD9-2372F90731E6}">
-  <dimension ref="A1"/>
+  <dimension ref="G1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G2" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="H2" s="2">
+        <v>-2.8</v>
+      </c>
+    </row>
+    <row r="3" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G3" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="H3" s="2">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G4" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="H4" s="2">
+        <v>-2.25</v>
+      </c>
+    </row>
+    <row r="5" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G5" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="H5" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="6" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G6" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>-1.75</v>
+      </c>
+    </row>
+    <row r="7" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G7" s="2">
+        <v>3</v>
+      </c>
+      <c r="H7" s="2">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="8" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G8" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="H8" s="2">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G9" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>-1.25</v>
+      </c>
+    </row>
+    <row r="10" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G10" s="2">
+        <v>2</v>
+      </c>
+      <c r="H10" s="2">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="11" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G11" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="H11" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G12" s="2">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H12" s="2">
+        <v>-0.75</v>
+      </c>
+    </row>
+    <row r="13" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <v>-0.66</v>
+      </c>
+    </row>
+    <row r="14" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G14" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="H14" s="2">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H15" s="2">
+        <v>-0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G16" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G17" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G18" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G19" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>